<commit_message>
readme update, ground truth files
</commit_message>
<xml_diff>
--- a/Evaluation table text_to_bpmn prompt 1 experiment 1 prompt 2 experiment 3.xlsx
+++ b/Evaluation table text_to_bpmn prompt 1 experiment 1 prompt 2 experiment 3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D Drive\Downloads\AGH\Winter Semester 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC1EC7F3-B3E2-4E1A-99D4-ABE698A343D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCBD4029-21F1-4518-9DAB-3CB075C8C315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{9F9EBB07-DFC8-4733-81BE-4BC402E9CB4E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{9F9EBB07-DFC8-4733-81BE-4BC402E9CB4E}"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="228">
   <si>
     <t>Relation type</t>
   </si>
@@ -709,6 +709,21 @@
   </si>
   <si>
     <t>repair finished</t>
+  </si>
+  <si>
+    <t>Task Recall</t>
+  </si>
+  <si>
+    <t>P1 Bing Baseline</t>
+  </si>
+  <si>
+    <t>P1 ChatGPT Baseline</t>
+  </si>
+  <si>
+    <t>P1 Gemini Baseline</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -904,7 +919,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -969,6 +984,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -981,31 +1008,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1085,6 +1088,56 @@
     <tableColumn id="2" xr3:uid="{6FB5C93D-AB7F-47EA-BF95-0813B529C8BF}" name="Author"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CDA04868-D1C0-4B33-9006-D3BE7EEBC42F}" name="Table1" displayName="Table1" ref="W21:AB24" totalsRowShown="0">
+  <autoFilter ref="W21:AB24" xr:uid="{CDA04868-D1C0-4B33-9006-D3BE7EEBC42F}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{5708538F-FBEF-4D28-B696-F8D1DF000C50}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{59062B9D-FB80-4F07-AF1D-53197273558E}" name="Friedrich et al.">
+      <calculatedColumnFormula>G36</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{B333EA11-FBD8-406E-BE75-94FFAD47E46D}" name="Grohs et al. Prompt 1 Try 1">
+      <calculatedColumnFormula>J36</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{B47F4DB2-7706-4C45-868B-353D291AC917}" name="P1 Bing Baseline">
+      <calculatedColumnFormula>M36</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{85F332F1-4F85-49D1-B721-D9CD4F700186}" name="P1 Gemini Baseline">
+      <calculatedColumnFormula>P36</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{D5CA4F27-6992-413B-8B27-66DFFA135BFE}" name="P1 ChatGPT Baseline">
+      <calculatedColumnFormula>S36</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A95088DB-6031-4B12-9E1E-9029F0394702}" name="Table16" displayName="Table16" ref="W17:AB20" totalsRowShown="0">
+  <autoFilter ref="W17:AB20" xr:uid="{A95088DB-6031-4B12-9E1E-9029F0394702}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{8141B549-D698-4C83-AB14-8C595738C497}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{82BC0141-6C41-4D8F-BC6A-7F63912E3B0E}" name="Friedrich et al.">
+      <calculatedColumnFormula>G19</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{E1A9F119-4FDE-40E1-9AEC-E4A9D6ECFFD2}" name="Grohs et al. Prompt 1 Try 1">
+      <calculatedColumnFormula>J19</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{55793D1A-00F4-441B-9410-013770E588B5}" name="P1 Bing Baseline">
+      <calculatedColumnFormula>M19</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{E77C5C78-C051-4821-8185-4504D6247D2B}" name="P1 Gemini Baseline">
+      <calculatedColumnFormula>P19</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{0070A681-B05E-4AE2-9E88-DDB6AD125A3D}" name="P1 ChatGPT Baseline">
+      <calculatedColumnFormula>S19</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1388,7 +1441,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,13 +1537,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB3172BA-7687-4430-A294-7BF072631175}">
-  <dimension ref="A1:U54"/>
+  <dimension ref="A1:AB54"/>
   <sheetViews>
-    <sheetView zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G26" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="53" zoomScaleNormal="53" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1:L1"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,42 +1562,49 @@
     <col min="18" max="18" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" customWidth="1"/>
+    <col min="23" max="23" width="11" customWidth="1"/>
+    <col min="24" max="24" width="16.140625" customWidth="1"/>
+    <col min="25" max="25" width="26.42578125" customWidth="1"/>
+    <col min="26" max="26" width="18.5703125" customWidth="1"/>
+    <col min="27" max="27" width="20.7109375" customWidth="1"/>
+    <col min="28" max="28" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="26" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="26" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="K1" s="27"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="26" t="s">
+      <c r="K1" s="31"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="N1" s="27"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="26" t="s">
+      <c r="N1" s="31"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="26" t="s">
+      <c r="Q1" s="31"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="T1" s="27"/>
-      <c r="U1" s="29"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="33"/>
     </row>
     <row r="2" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -2412,7 +2472,7 @@
       <c r="T16" s="9"/>
       <c r="U16" s="20"/>
     </row>
-    <row r="17" spans="1:21" ht="150" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2462,7 +2522,7 @@
       <c r="T17" s="9"/>
       <c r="U17" s="20"/>
     </row>
-    <row r="18" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2528,7 +2588,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2578,7 +2638,7 @@
       <c r="T19" s="9"/>
       <c r="U19" s="20"/>
     </row>
-    <row r="20" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2624,7 +2684,7 @@
       <c r="T20" s="9"/>
       <c r="U20" s="20"/>
     </row>
-    <row r="21" spans="1:21" ht="105" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2677,8 +2737,26 @@
       </c>
       <c r="T21" s="9"/>
       <c r="U21" s="20"/>
-    </row>
-    <row r="22" spans="1:21" ht="105" x14ac:dyDescent="0.25">
+      <c r="W21" t="s">
+        <v>227</v>
+      </c>
+      <c r="X21" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>224</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>226</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2731,8 +2809,31 @@
       </c>
       <c r="T22" s="9"/>
       <c r="U22" s="20"/>
-    </row>
-    <row r="23" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="W22" t="s">
+        <v>223</v>
+      </c>
+      <c r="X22">
+        <f>G29</f>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="Y22">
+        <f>J29</f>
+        <v>0.46153846153846156</v>
+      </c>
+      <c r="Z22">
+        <f>M29</f>
+        <v>0.57692307692307687</v>
+      </c>
+      <c r="AA22">
+        <f>P29</f>
+        <v>0.65384615384615385</v>
+      </c>
+      <c r="AB22">
+        <f>S29</f>
+        <v>0.45454545454545453</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2775,8 +2876,31 @@
       <c r="S23" s="9"/>
       <c r="T23" s="9"/>
       <c r="U23" s="20"/>
-    </row>
-    <row r="24" spans="1:21" ht="150" x14ac:dyDescent="0.25">
+      <c r="W23" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="X23">
+        <f>G37</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="Y23">
+        <f>J37</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="Z23">
+        <f>M37</f>
+        <v>1</v>
+      </c>
+      <c r="AA23">
+        <f>P37</f>
+        <v>1</v>
+      </c>
+      <c r="AB23">
+        <f>S37</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2823,8 +2947,31 @@
       <c r="S24" s="9"/>
       <c r="T24" s="9"/>
       <c r="U24" s="20"/>
-    </row>
-    <row r="25" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="W24" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="X24">
+        <f>G38</f>
+        <v>0.48484848484848486</v>
+      </c>
+      <c r="Y24">
+        <f>J38</f>
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="Z24">
+        <f>M38</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AA24">
+        <f>P38</f>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="AB24">
+        <f>S38</f>
+        <v>0.58620689655172409</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2868,7 +3015,7 @@
       <c r="T25" s="9"/>
       <c r="U25" s="20"/>
     </row>
-    <row r="26" spans="1:21" ht="150" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2926,7 +3073,7 @@
       <c r="T26" s="9"/>
       <c r="U26" s="20"/>
     </row>
-    <row r="27" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2988,7 +3135,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -3044,7 +3191,7 @@
       <c r="T28" s="9"/>
       <c r="U28" s="20"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="10"/>
       <c r="C29" s="9"/>
@@ -3053,38 +3200,38 @@
       <c r="F29" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="G29" s="36">
+      <c r="G29" s="28">
         <f>SUM(G3:G28)/COUNT(G3:G28)</f>
         <v>0.38461538461538464</v>
       </c>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="36">
+      <c r="J29" s="28">
         <f>SUM(J3:J28)/COUNT(J3:J28)</f>
         <v>0.46153846153846156</v>
       </c>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
-      <c r="M29" s="36">
+      <c r="M29" s="28">
         <f>SUM(M3:M28)/COUNT(M3:M28)</f>
         <v>0.57692307692307687</v>
       </c>
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
-      <c r="P29" s="36">
+      <c r="P29" s="28">
         <f>SUM(P3:P28)/COUNT(P3:P28)</f>
         <v>0.65384615384615385</v>
       </c>
       <c r="Q29" s="9"/>
       <c r="R29" s="20"/>
-      <c r="S29" s="37">
+      <c r="S29" s="29">
         <f>SUM(S3:S28)/COUNT(S3:S28)</f>
         <v>0.45454545454545453</v>
       </c>
       <c r="T29" s="9"/>
       <c r="U29" s="20"/>
     </row>
-    <row r="30" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>1</v>
       </c>
@@ -3145,7 +3292,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>1+A30</f>
         <v>2</v>
@@ -3203,7 +3350,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" ref="A32:A36" si="2">1+A31</f>
         <v>3</v>
@@ -3648,6 +3795,9 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -3656,13 +3806,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:AB36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O3" sqref="O3"/>
+      <selection pane="bottomRight" activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3688,38 +3838,38 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="26" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="26" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="30" t="s">
         <v>214</v>
       </c>
-      <c r="K1" s="27"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="26" t="s">
+      <c r="K1" s="31"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="30" t="s">
         <v>205</v>
       </c>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="26" t="s">
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="30" t="s">
         <v>206</v>
       </c>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="26" t="s">
+      <c r="Q1" s="31"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="T1" s="27"/>
-      <c r="U1" s="28"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="32"/>
     </row>
     <row r="2" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -3787,52 +3937,47 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="31">
-        <v>1</v>
-      </c>
-      <c r="B3" s="32" t="s">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="9" t="s">
         <v>146</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="32">
-        <v>1</v>
-      </c>
-      <c r="H3" s="31" t="s">
+      <c r="G3" s="10">
+        <v>1</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>146</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="J3" s="32">
-        <v>0</v>
-      </c>
-      <c r="K3" s="31"/>
-      <c r="M3" s="32">
-        <v>0</v>
-      </c>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
+      <c r="J3" s="10">
+        <v>0</v>
+      </c>
+      <c r="M3" s="10">
+        <v>0</v>
+      </c>
       <c r="P3" s="10">
         <v>0</v>
       </c>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="34">
-        <v>0</v>
-      </c>
-      <c r="T3" s="34"/>
-      <c r="U3" s="38"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="9">
+        <v>0</v>
+      </c>
+      <c r="U3" s="20"/>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -4078,7 +4223,7 @@
       <c r="C9" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="9" t="s">
         <v>93</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -4186,19 +4331,19 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G11" s="10">
@@ -4270,7 +4415,7 @@
       <c r="B13" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="9" t="s">
         <v>202</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -4308,10 +4453,10 @@
       <c r="B14" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="9" t="s">
         <v>102</v>
       </c>
       <c r="E14" s="9" t="s">
@@ -4346,10 +4491,10 @@
       <c r="B15" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="9" t="s">
         <v>199</v>
       </c>
       <c r="E15" s="9" t="s">
@@ -4395,16 +4540,16 @@
       <c r="B16" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="9" t="s">
         <v>102</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G16" s="10">
@@ -4448,24 +4593,24 @@
       </c>
       <c r="U16" s="20"/>
     </row>
-    <row r="17" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="33" t="s">
+      <c r="F17" s="11" t="s">
         <v>200</v>
       </c>
       <c r="G17" s="10">
@@ -4485,25 +4630,43 @@
         <v>0</v>
       </c>
       <c r="U17" s="20"/>
-    </row>
-    <row r="18" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="W17" t="s">
+        <v>227</v>
+      </c>
+      <c r="X17" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>224</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>226</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="F18" s="11" t="s">
         <v>19</v>
       </c>
       <c r="G18" s="10">
@@ -4523,25 +4686,48 @@
         <v>0</v>
       </c>
       <c r="U18" s="20"/>
-    </row>
-    <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="W18" t="s">
+        <v>223</v>
+      </c>
+      <c r="X18">
+        <f>G25</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="Y18">
+        <f>J25</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="Z18">
+        <f>M25</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="AA18">
+        <f>P25</f>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="AB18">
+        <f>S25</f>
+        <v>0.22727272727272727</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="9" t="s">
         <v>201</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="F19" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G19" s="10">
@@ -4561,8 +4747,31 @@
         <v>0</v>
       </c>
       <c r="U19" s="20"/>
-    </row>
-    <row r="20" spans="1:21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="W19" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="X19">
+        <f>G33</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="Y19">
+        <f>J33</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="Z19">
+        <f>M33</f>
+        <v>1</v>
+      </c>
+      <c r="AA19">
+        <f>P33</f>
+        <v>1</v>
+      </c>
+      <c r="AB19">
+        <f>S33</f>
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -4619,25 +4828,48 @@
       </c>
       <c r="T20" s="9"/>
       <c r="U20" s="20"/>
-    </row>
-    <row r="21" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="W20" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="X20">
+        <f>G34</f>
+        <v>0.2413793103448276</v>
+      </c>
+      <c r="Y20">
+        <f>J34</f>
+        <v>0.37037037037037035</v>
+      </c>
+      <c r="Z20">
+        <f>M34</f>
+        <v>0.51724137931034486</v>
+      </c>
+      <c r="AA20">
+        <f>P34</f>
+        <v>0.44827586206896552</v>
+      </c>
+      <c r="AB20">
+        <f>S34</f>
+        <v>0.31034482758620691</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G21" s="10">
@@ -4675,24 +4907,24 @@
       </c>
       <c r="U21" s="20"/>
     </row>
-    <row r="22" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="11" t="s">
         <v>19</v>
       </c>
       <c r="G22" s="10">
@@ -4713,24 +4945,24 @@
       </c>
       <c r="U22" s="20"/>
     </row>
-    <row r="23" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="11" t="s">
         <v>19</v>
       </c>
       <c r="G23" s="10">
@@ -4751,18 +4983,18 @@
       </c>
       <c r="U23" s="20"/>
     </row>
-    <row r="24" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="9" t="s">
         <v>102</v>
       </c>
       <c r="E24" s="9" t="s">
@@ -4789,35 +5021,35 @@
       </c>
       <c r="U24" s="20"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="F25" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="G25" s="30">
+      <c r="G25" s="26">
         <f>SUM(G3:G24)/COUNT(G3:G24)</f>
         <v>0.18181818181818182</v>
       </c>
-      <c r="J25" s="30">
+      <c r="J25" s="26">
         <f>SUM(J3:J24)/COUNT(J3:J24)</f>
         <v>0.2857142857142857</v>
       </c>
-      <c r="M25" s="30">
+      <c r="M25" s="26">
         <f>SUM(M3:M24)/COUNT(M3:M24)</f>
         <v>0.36363636363636365</v>
       </c>
-      <c r="P25" s="30">
+      <c r="P25" s="26">
         <f>SUM(P3:P24)/COUNT(P3:P24)</f>
         <v>0.27272727272727271</v>
       </c>
       <c r="R25" s="20"/>
-      <c r="S25" s="30">
+      <c r="S25" s="26">
         <f>SUM(S3:S24)/COUNT(S3:S24)</f>
         <v>0.22727272727272727</v>
       </c>
       <c r="U25" s="20"/>
     </row>
-    <row r="26" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>1</v>
       </c>
@@ -4866,7 +5098,7 @@
       </c>
       <c r="U26" s="20"/>
     </row>
-    <row r="27" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <f>1+A26</f>
         <v>2</v>
@@ -4927,7 +5159,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -4982,7 +5214,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -5029,7 +5261,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -5084,7 +5316,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -5134,7 +5366,7 @@
       </c>
       <c r="U31" s="20"/>
     </row>
-    <row r="32" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -5142,7 +5374,7 @@
       <c r="B32" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="27" t="s">
         <v>193</v>
       </c>
       <c r="D32" s="9" t="s">
@@ -5155,7 +5387,7 @@
       <c r="J32" s="10">
         <v>1</v>
       </c>
-      <c r="K32" s="35" t="s">
+      <c r="K32" s="27" t="s">
         <v>193</v>
       </c>
       <c r="L32" s="9" t="s">
@@ -5164,7 +5396,7 @@
       <c r="M32" s="10">
         <v>1</v>
       </c>
-      <c r="N32" s="35" t="s">
+      <c r="N32" s="27" t="s">
         <v>193</v>
       </c>
       <c r="O32" s="9" t="s">
@@ -5173,7 +5405,7 @@
       <c r="P32" s="10">
         <v>1</v>
       </c>
-      <c r="Q32" s="35" t="s">
+      <c r="Q32" s="27" t="s">
         <v>193</v>
       </c>
       <c r="R32" s="20" t="s">
@@ -5182,7 +5414,7 @@
       <c r="S32" s="10">
         <v>0</v>
       </c>
-      <c r="T32" s="35"/>
+      <c r="T32" s="27"/>
       <c r="U32" s="20"/>
     </row>
     <row r="33" spans="2:21" x14ac:dyDescent="0.25">
@@ -5290,7 +5522,10 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
-  <pageSetup scale="39" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="23" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -5331,43 +5566,43 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="26" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="26" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="26" t="s">
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="27"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="26" t="s">
+      <c r="N1" s="31"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="26" t="s">
+      <c r="Q1" s="31"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="26" t="s">
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
     </row>
     <row r="2" spans="1:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -6941,43 +7176,43 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="26" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="26" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="26" t="s">
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="27"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="26" t="s">
+      <c r="N1" s="31"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="26" t="s">
+      <c r="Q1" s="31"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="26" t="s">
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
     </row>
     <row r="2" spans="1:24" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -8405,6 +8640,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100FF1B78D5E9E25C4C840B53239D764C24" ma:contentTypeVersion="16" ma:contentTypeDescription="Utwórz nowy dokument." ma:contentTypeScope="" ma:versionID="746ce095a376785e56f8e1418f7e1413">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c8f656d6-3613-40d7-a283-9b9e2fc0b499" xmlns:ns4="84bae827-43eb-4799-b986-0b4b10c2bedf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="08323d50b603442337e480d3a3ca5dcf" ns3:_="" ns4:_="">
     <xsd:import namespace="c8f656d6-3613-40d7-a283-9b9e2fc0b499"/>
@@ -8645,15 +8889,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -8663,6 +8898,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F734B24B-2C24-467A-8687-B2C54676852F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFC546EE-5936-468C-83D0-058F0B36004C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8681,27 +8924,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F734B24B-2C24-467A-8687-B2C54676852F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16DAB4F2-D0DD-443F-BBD6-5C7CC329DA2C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c8f656d6-3613-40d7-a283-9b9e2fc0b499"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="c8f656d6-3613-40d7-a283-9b9e2fc0b499"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="84bae827-43eb-4799-b986-0b4b10c2bedf"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>